<commit_message>
Modify Excel workbook to pivot data into more easily digested rows and columns
Also, add readme worksheet
</commit_message>
<xml_diff>
--- a/Post2026WebTool/DMDU-Performance.xlsx
+++ b/Post2026WebTool/DMDU-Performance.xlsx
@@ -5,17 +5,22 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Box\ColoradoRiver\Reclamation-DMDU-Tool\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCollaborate\Post2026WebTool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E258F68-00BB-4909-A8DD-143EC651755E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F9FB718-240D-4530-8BA8-8867CC570D29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5F776126-F472-4954-8F54-2D1027C60DF9}"/>
+    <workbookView xWindow="-57720" yWindow="-1800" windowWidth="29040" windowHeight="17520" xr2:uid="{5F776126-F472-4954-8F54-2D1027C60DF9}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="ReadMe" sheetId="3" r:id="rId1"/>
+    <sheet name="PivotTable" sheetId="2" r:id="rId2"/>
+    <sheet name="Data" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <pivotCaches>
+    <pivotCache cacheId="13" r:id="rId4"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,15 +41,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="22">
   <si>
     <t>Hydrology</t>
   </si>
   <si>
     <t>Strategy ID</t>
-  </si>
-  <si>
-    <t>GCD Release Minimum (maf)</t>
   </si>
   <si>
     <t>Late 20230s Drought</t>
@@ -65,7 +67,46 @@
     <t>Default optimization</t>
   </si>
   <si>
-    <t>Powell &lt; 3,490 feet (%)</t>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>Powell &lt; 3,490 feet (% of Months)</t>
+  </si>
+  <si>
+    <t>GCD Minimum Annual Release (maf)</t>
+  </si>
+  <si>
+    <t>Sum of Powell &lt; 3,490 feet (% of Months)</t>
+  </si>
+  <si>
+    <t>Sum of GCD Minimum Annual Release (maf)</t>
+  </si>
+  <si>
+    <t>Reclamation's Post 2026 Web Tool</t>
+  </si>
+  <si>
+    <t>Worksheet</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Raw data of Hydrology  Ensamble, Alternative, Percent of Months below 3,490 feet, and minimum annual rease. These values are copied from the ____ Tab within the webtool.</t>
+  </si>
+  <si>
+    <t>PivotTable</t>
+  </si>
+  <si>
+    <t>An Excel Pivot table that presents the data in Alternative/ Hydrology (Rows) and Percent of Months and Minimum Annual Flow (Columns)</t>
+  </si>
+  <si>
+    <t>This workbook summarizes analysis in Reclamations Post-2026 Operations Exploration Tool with the goal to identify minimum Glen Canyon Dam annual releases needed to protect Lake Powell from drawdown below elevations 3,490 feet (Minimum power pool) and 3,525 feet (Protection elevation defined in the 2019 Drought Contingency Plan).</t>
+  </si>
+  <si>
+    <t>See ReadMe.md document for further elaboration and directions to reproduce results.</t>
   </si>
 </sst>
 </file>
@@ -109,7 +150,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -117,11 +158,114 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="24">
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -132,6 +276,564 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="david" refreshedDate="45586.516571874999" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="36" xr:uid="{1714E6C7-A833-4DC5-A6A0-4971455C5CC2}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:D37" sheet="Data"/>
+  </cacheSource>
+  <cacheFields count="4">
+    <cacheField name="Hydrology" numFmtId="0">
+      <sharedItems count="6">
+        <s v="Late 20230s Drought"/>
+        <s v="11 maf, infrequent high flows"/>
+        <s v="Early High Flows, then 12 maf"/>
+        <s v="Decreasing Trend from 12 to 10 maf"/>
+        <s v="Drought through 2028 then 11.5 maf"/>
+        <s v="Default optimization"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Strategy ID" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="26992" maxValue="98230" count="6">
+        <n v="85558"/>
+        <n v="49068"/>
+        <n v="89269"/>
+        <n v="98230"/>
+        <n v="95580"/>
+        <n v="26992"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Powell &lt; 3,490 feet (% of Months)" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0" maxValue="3" count="7">
+        <n v="0"/>
+        <n v="0.1"/>
+        <n v="0.3"/>
+        <n v="0.5"/>
+        <n v="0.8"/>
+        <n v="3"/>
+        <n v="1"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="GCD Minimum Annual Release (maf)" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="3.96" maxValue="6.45" count="30">
+        <n v="6"/>
+        <n v="4.59"/>
+        <n v="4.41"/>
+        <n v="4.2699999999999996"/>
+        <n v="3.96"/>
+        <n v="5.94"/>
+        <n v="5.16"/>
+        <n v="4.74"/>
+        <n v="4.12"/>
+        <n v="4.75"/>
+        <n v="4.4400000000000004"/>
+        <n v="4.1100000000000003"/>
+        <n v="5.15"/>
+        <n v="5.69"/>
+        <n v="5.77"/>
+        <n v="4.4000000000000004"/>
+        <n v="3.97"/>
+        <n v="4.6100000000000003"/>
+        <n v="4.71"/>
+        <n v="5.57"/>
+        <n v="5.53"/>
+        <n v="5.85"/>
+        <n v="4.6900000000000004"/>
+        <n v="5.12"/>
+        <n v="4.68"/>
+        <n v="4.1900000000000004"/>
+        <n v="6.03"/>
+        <n v="6.45"/>
+        <n v="5.41"/>
+        <n v="4.4800000000000004"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="36">
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="8"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="9"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="10"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="11"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="12"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="3"/>
+    <x v="13"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="4"/>
+    <x v="14"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="15"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="16"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="17"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="18"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="19"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="5"/>
+    <x v="20"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="1"/>
+    <x v="6"/>
+    <x v="21"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="22"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="23"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="21"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="24"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="25"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="26"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="27"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="28"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="29"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00E99385-38E0-4A97-8334-300435782A5C}" name="PivotTable1" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:C45" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="4">
+    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
+      <items count="6">
+        <item x="1"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item x="5"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
+      <items count="6">
+        <item x="5"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item x="1"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0">
+      <items count="7">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="6"/>
+        <item x="5"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0">
+      <items count="30">
+        <item x="4"/>
+        <item x="16"/>
+        <item x="11"/>
+        <item x="8"/>
+        <item x="25"/>
+        <item x="3"/>
+        <item x="15"/>
+        <item x="2"/>
+        <item x="10"/>
+        <item x="29"/>
+        <item x="1"/>
+        <item x="17"/>
+        <item x="24"/>
+        <item x="22"/>
+        <item x="18"/>
+        <item x="7"/>
+        <item x="9"/>
+        <item x="23"/>
+        <item x="12"/>
+        <item x="6"/>
+        <item x="28"/>
+        <item x="20"/>
+        <item x="19"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="21"/>
+        <item x="5"/>
+        <item x="0"/>
+        <item x="26"/>
+        <item x="27"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="1"/>
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="42">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Powell &lt; 3,490 feet (% of Months)" fld="2" baseField="0" baseItem="0"/>
+    <dataField name="Sum of GCD Minimum Annual Release (maf)" fld="3" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="4">
+    <format dxfId="23">
+      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="22">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="2">
+            <x v="0"/>
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="21">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="20">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="2">
+            <x v="0"/>
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -450,11 +1152,590 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDE794B6-A7D0-4151-B3B3-0A01917D1254}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.453125" style="11" customWidth="1"/>
+    <col min="2" max="2" width="58.54296875" style="10" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="87" x14ac:dyDescent="0.35">
+      <c r="B3" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="B4" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A8" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADA64DF2-8BDA-4183-86B2-4FB89DC77176}">
+  <dimension ref="A3:AG45"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="34.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.36328125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="15.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="4.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="28" width="4.81640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="3.81640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="33" width="4.81640625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="19.90625" bestFit="1" customWidth="1"/>
+    <col min="35" max="37" width="4.81640625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="1.90625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="23.1796875" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="8" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="5.54296875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="8" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="5.54296875" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="8" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="31.08984375" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="19.90625" bestFit="1" customWidth="1"/>
+    <col min="48" max="50" width="4.81640625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="1.90625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="6.54296875" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="23.1796875" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="10.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:33" s="4" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="3">
+        <v>26992</v>
+      </c>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4"/>
+      <c r="E4"/>
+      <c r="F4"/>
+      <c r="G4"/>
+      <c r="H4"/>
+      <c r="I4"/>
+      <c r="J4"/>
+      <c r="K4"/>
+      <c r="L4"/>
+      <c r="M4"/>
+      <c r="N4"/>
+      <c r="O4"/>
+      <c r="P4"/>
+      <c r="Q4"/>
+      <c r="R4"/>
+      <c r="S4"/>
+      <c r="T4"/>
+      <c r="U4"/>
+      <c r="V4"/>
+      <c r="W4"/>
+      <c r="X4"/>
+      <c r="Y4"/>
+      <c r="Z4"/>
+      <c r="AA4"/>
+      <c r="AB4"/>
+      <c r="AC4"/>
+      <c r="AD4"/>
+      <c r="AE4"/>
+      <c r="AF4"/>
+      <c r="AG4"/>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="8">
+        <v>0</v>
+      </c>
+      <c r="C5" s="8">
+        <v>4.12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="8">
+        <v>0</v>
+      </c>
+      <c r="C6" s="8">
+        <v>3.97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="8">
+        <v>0</v>
+      </c>
+      <c r="C7" s="8">
+        <v>4.1900000000000004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A8" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="8">
+        <v>0</v>
+      </c>
+      <c r="C8" s="8">
+        <v>4.1100000000000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A9" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="8">
+        <v>0</v>
+      </c>
+      <c r="C9" s="8">
+        <v>3.96</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="8">
+        <v>0</v>
+      </c>
+      <c r="C10" s="8">
+        <v>4.4800000000000004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A11" s="3">
+        <v>95580</v>
+      </c>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A12" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="8">
+        <v>0</v>
+      </c>
+      <c r="C12" s="8">
+        <v>4.74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A13" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="8">
+        <v>0</v>
+      </c>
+      <c r="C13" s="8">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A14" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="8">
+        <v>0</v>
+      </c>
+      <c r="C14" s="8">
+        <v>4.68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A15" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="8">
+        <v>0</v>
+      </c>
+      <c r="C15" s="8">
+        <v>4.4400000000000004</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A16" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="8">
+        <v>0</v>
+      </c>
+      <c r="C16" s="8">
+        <v>4.2699999999999996</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="8">
+        <v>0</v>
+      </c>
+      <c r="C17" s="8">
+        <v>5.41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" s="3">
+        <v>98230</v>
+      </c>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="8">
+        <v>0</v>
+      </c>
+      <c r="C19" s="8">
+        <v>4.74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="C20" s="8">
+        <v>4.6100000000000003</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="8">
+        <v>0</v>
+      </c>
+      <c r="C21" s="8">
+        <v>4.6900000000000004</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="8">
+        <v>0</v>
+      </c>
+      <c r="C22" s="8">
+        <v>4.75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" s="8">
+        <v>0</v>
+      </c>
+      <c r="C23" s="8">
+        <v>4.41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="8">
+        <v>0</v>
+      </c>
+      <c r="C24" s="8">
+        <v>6.03</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" s="3">
+        <v>89269</v>
+      </c>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26" s="8">
+        <v>0</v>
+      </c>
+      <c r="C26" s="8">
+        <v>5.16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="C27" s="8">
+        <v>4.71</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="8">
+        <v>0</v>
+      </c>
+      <c r="C28" s="8">
+        <v>5.12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29" s="8">
+        <v>0.3</v>
+      </c>
+      <c r="C29" s="8">
+        <v>5.15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B30" s="8">
+        <v>0</v>
+      </c>
+      <c r="C30" s="8">
+        <v>4.59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31" s="8">
+        <v>0</v>
+      </c>
+      <c r="C31" s="8">
+        <v>6.45</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" s="3">
+        <v>85558</v>
+      </c>
+      <c r="B32" s="8"/>
+      <c r="C32" s="8"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33" s="8">
+        <v>0</v>
+      </c>
+      <c r="C33" s="8">
+        <v>5.94</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="C34" s="8">
+        <v>5.57</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="8">
+        <v>0</v>
+      </c>
+      <c r="C35" s="8">
+        <v>5.85</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B36" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="C36" s="8">
+        <v>5.69</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B37" s="8">
+        <v>0</v>
+      </c>
+      <c r="C37" s="8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38" s="8">
+        <v>0</v>
+      </c>
+      <c r="C38" s="8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39" s="3">
+        <v>49068</v>
+      </c>
+      <c r="B39" s="8"/>
+      <c r="C39" s="8"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A40" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B40" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="C40" s="8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A41" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B41" s="8">
+        <v>3</v>
+      </c>
+      <c r="C41" s="8">
+        <v>5.53</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A42" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B42" s="8">
+        <v>1</v>
+      </c>
+      <c r="C42" s="8">
+        <v>5.85</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A43" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B43" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="C43" s="8">
+        <v>5.77</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A44" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B44" s="8">
+        <v>0</v>
+      </c>
+      <c r="C44" s="8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A45" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B45" s="8">
+        <v>0</v>
+      </c>
+      <c r="C45" s="8">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4303D6EF-8192-42ED-A171-03A91BCCA98D}">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -465,7 +1746,7 @@
     <col min="4" max="4" width="11.90625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="87" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -476,12 +1757,12 @@
         <v>9</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" s="2">
         <v>85558</v>
@@ -495,7 +1776,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="2">
         <v>49068</v>
@@ -509,7 +1790,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="2">
         <v>89269</v>
@@ -523,7 +1804,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" s="2">
         <v>98230</v>
@@ -537,7 +1818,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B6" s="2">
         <v>95580</v>
@@ -551,7 +1832,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B7" s="2">
         <v>26992</v>
@@ -565,7 +1846,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B8" s="2">
         <v>49068</v>
@@ -579,7 +1860,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B9" s="2">
         <v>85558</v>
@@ -593,7 +1874,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B10" s="2">
         <v>89269</v>
@@ -607,7 +1888,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B11" s="2">
         <v>98230</v>
@@ -621,7 +1902,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B12" s="2">
         <v>95580</v>
@@ -635,7 +1916,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B13" s="2">
         <v>26992</v>
@@ -649,7 +1930,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B14" s="2">
         <v>98230</v>
@@ -663,7 +1944,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B15" s="2">
         <v>95580</v>
@@ -677,7 +1958,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B16" s="2">
         <v>26992</v>
@@ -691,7 +1972,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B17" s="2">
         <v>89269</v>
@@ -705,7 +1986,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B18" s="2">
         <v>85558</v>
@@ -719,7 +2000,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B19" s="2">
         <v>49068</v>
@@ -733,7 +2014,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B20" s="2">
         <v>95580</v>
@@ -747,7 +2028,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B21" s="2">
         <v>26992</v>
@@ -761,7 +2042,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B22" s="2">
         <v>98230</v>
@@ -775,7 +2056,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B23" s="2">
         <v>89269</v>
@@ -789,7 +2070,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B24" s="2">
         <v>85558</v>
@@ -803,7 +2084,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B25" s="2">
         <v>49068</v>
@@ -817,7 +2098,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B26" s="2">
         <v>49068</v>
@@ -831,7 +2112,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B27" s="2">
         <v>98230</v>
@@ -845,7 +2126,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B28" s="2">
         <v>89269</v>
@@ -859,7 +2140,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B29" s="2">
         <v>85558</v>
@@ -873,7 +2154,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B30" s="2">
         <v>95580</v>
@@ -887,7 +2168,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B31" s="2">
         <v>26992</v>
@@ -901,7 +2182,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B32" s="2">
         <v>98230</v>
@@ -915,7 +2196,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B33" s="2">
         <v>89269</v>
@@ -929,7 +2210,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B34" s="2">
         <v>85558</v>
@@ -943,7 +2224,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B35" s="2">
         <v>49068</v>
@@ -957,7 +2238,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B36" s="2">
         <v>95580</v>
@@ -971,7 +2252,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B37" s="2">
         <v>26992</v>

</xml_diff>

<commit_message>
Start ReadMe.md tile and move old sessions to separate folder
</commit_message>
<xml_diff>
--- a/Post2026WebTool/DMDU-Performance.xlsx
+++ b/Post2026WebTool/DMDU-Performance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCollaborate\Post2026WebTool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F9FB718-240D-4530-8BA8-8867CC570D29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B25A27C9-1FF9-4838-9FB0-7B86A90BF17E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57720" yWindow="-1800" windowWidth="29040" windowHeight="17520" xr2:uid="{5F776126-F472-4954-8F54-2D1027C60DF9}"/>
+    <workbookView xWindow="-57720" yWindow="-1800" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{5F776126-F472-4954-8F54-2D1027C60DF9}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="3" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="13" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -150,7 +150,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -173,9 +173,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -192,67 +189,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <alignment horizontal="center"/>
     </dxf>
@@ -580,7 +517,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00E99385-38E0-4A97-8334-300435782A5C}" name="PivotTable1" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00E99385-38E0-4A97-8334-300435782A5C}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C45" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
@@ -797,10 +734,10 @@
     <dataField name="Sum of GCD Minimum Annual Release (maf)" fld="3" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="4">
-    <format dxfId="23">
+    <format dxfId="3">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="22">
+    <format dxfId="2">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="2">
@@ -810,10 +747,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="21">
+    <format dxfId="1">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="20">
+    <format dxfId="0">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="2">
@@ -1155,52 +1092,52 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDE794B6-A7D0-4151-B3B3-0A01917D1254}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.453125" style="11" customWidth="1"/>
-    <col min="2" max="2" width="58.54296875" style="10" customWidth="1"/>
+    <col min="1" max="1" width="10.453125" style="10" customWidth="1"/>
+    <col min="2" max="2" width="58.54296875" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="87" x14ac:dyDescent="0.35">
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="11" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="9" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="9" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1213,8 +1150,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADA64DF2-8BDA-4183-86B2-4FB89DC77176}">
   <dimension ref="A3:AG45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1261,8 +1198,8 @@
       <c r="A4" s="3">
         <v>26992</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
       <c r="D4"/>
       <c r="E4"/>
       <c r="F4"/>
@@ -1298,10 +1235,10 @@
       <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="8">
-        <v>0</v>
-      </c>
-      <c r="C5" s="8">
+      <c r="B5" s="2">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2">
         <v>4.12</v>
       </c>
     </row>
@@ -1309,10 +1246,10 @@
       <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="8">
-        <v>0</v>
-      </c>
-      <c r="C6" s="8">
+      <c r="B6" s="2">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2">
         <v>3.97</v>
       </c>
     </row>
@@ -1320,10 +1257,10 @@
       <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="8">
-        <v>0</v>
-      </c>
-      <c r="C7" s="8">
+      <c r="B7" s="2">
+        <v>0</v>
+      </c>
+      <c r="C7" s="2">
         <v>4.1900000000000004</v>
       </c>
     </row>
@@ -1331,10 +1268,10 @@
       <c r="A8" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="8">
-        <v>0</v>
-      </c>
-      <c r="C8" s="8">
+      <c r="B8" s="2">
+        <v>0</v>
+      </c>
+      <c r="C8" s="2">
         <v>4.1100000000000003</v>
       </c>
     </row>
@@ -1342,10 +1279,10 @@
       <c r="A9" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="8">
-        <v>0</v>
-      </c>
-      <c r="C9" s="8">
+      <c r="B9" s="2">
+        <v>0</v>
+      </c>
+      <c r="C9" s="2">
         <v>3.96</v>
       </c>
     </row>
@@ -1353,10 +1290,10 @@
       <c r="A10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="8">
-        <v>0</v>
-      </c>
-      <c r="C10" s="8">
+      <c r="B10" s="2">
+        <v>0</v>
+      </c>
+      <c r="C10" s="2">
         <v>4.4800000000000004</v>
       </c>
     </row>
@@ -1364,17 +1301,15 @@
       <c r="A11" s="3">
         <v>95580</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="8">
-        <v>0</v>
-      </c>
-      <c r="C12" s="8">
+      <c r="B12" s="2">
+        <v>0</v>
+      </c>
+      <c r="C12" s="2">
         <v>4.74</v>
       </c>
     </row>
@@ -1382,10 +1317,10 @@
       <c r="A13" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="8">
-        <v>0</v>
-      </c>
-      <c r="C13" s="8">
+      <c r="B13" s="2">
+        <v>0</v>
+      </c>
+      <c r="C13" s="2">
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -1393,10 +1328,10 @@
       <c r="A14" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="8">
-        <v>0</v>
-      </c>
-      <c r="C14" s="8">
+      <c r="B14" s="2">
+        <v>0</v>
+      </c>
+      <c r="C14" s="2">
         <v>4.68</v>
       </c>
     </row>
@@ -1404,10 +1339,10 @@
       <c r="A15" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="8">
-        <v>0</v>
-      </c>
-      <c r="C15" s="8">
+      <c r="B15" s="2">
+        <v>0</v>
+      </c>
+      <c r="C15" s="2">
         <v>4.4400000000000004</v>
       </c>
     </row>
@@ -1415,10 +1350,10 @@
       <c r="A16" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="8">
-        <v>0</v>
-      </c>
-      <c r="C16" s="8">
+      <c r="B16" s="2">
+        <v>0</v>
+      </c>
+      <c r="C16" s="2">
         <v>4.2699999999999996</v>
       </c>
     </row>
@@ -1426,10 +1361,10 @@
       <c r="A17" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="8">
-        <v>0</v>
-      </c>
-      <c r="C17" s="8">
+      <c r="B17" s="2">
+        <v>0</v>
+      </c>
+      <c r="C17" s="2">
         <v>5.41</v>
       </c>
     </row>
@@ -1437,17 +1372,15 @@
       <c r="A18" s="3">
         <v>98230</v>
       </c>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B19" s="8">
-        <v>0</v>
-      </c>
-      <c r="C19" s="8">
+      <c r="B19" s="2">
+        <v>0</v>
+      </c>
+      <c r="C19" s="2">
         <v>4.74</v>
       </c>
     </row>
@@ -1455,10 +1388,10 @@
       <c r="A20" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B20" s="8">
+      <c r="B20" s="2">
         <v>0.1</v>
       </c>
-      <c r="C20" s="8">
+      <c r="C20" s="2">
         <v>4.6100000000000003</v>
       </c>
     </row>
@@ -1466,10 +1399,10 @@
       <c r="A21" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="8">
-        <v>0</v>
-      </c>
-      <c r="C21" s="8">
+      <c r="B21" s="2">
+        <v>0</v>
+      </c>
+      <c r="C21" s="2">
         <v>4.6900000000000004</v>
       </c>
     </row>
@@ -1477,10 +1410,10 @@
       <c r="A22" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B22" s="8">
-        <v>0</v>
-      </c>
-      <c r="C22" s="8">
+      <c r="B22" s="2">
+        <v>0</v>
+      </c>
+      <c r="C22" s="2">
         <v>4.75</v>
       </c>
     </row>
@@ -1488,10 +1421,10 @@
       <c r="A23" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="8">
-        <v>0</v>
-      </c>
-      <c r="C23" s="8">
+      <c r="B23" s="2">
+        <v>0</v>
+      </c>
+      <c r="C23" s="2">
         <v>4.41</v>
       </c>
     </row>
@@ -1499,10 +1432,10 @@
       <c r="A24" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B24" s="8">
-        <v>0</v>
-      </c>
-      <c r="C24" s="8">
+      <c r="B24" s="2">
+        <v>0</v>
+      </c>
+      <c r="C24" s="2">
         <v>6.03</v>
       </c>
     </row>
@@ -1510,17 +1443,15 @@
       <c r="A25" s="3">
         <v>89269</v>
       </c>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B26" s="8">
-        <v>0</v>
-      </c>
-      <c r="C26" s="8">
+      <c r="B26" s="2">
+        <v>0</v>
+      </c>
+      <c r="C26" s="2">
         <v>5.16</v>
       </c>
     </row>
@@ -1528,10 +1459,10 @@
       <c r="A27" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B27" s="8">
+      <c r="B27" s="2">
         <v>0.1</v>
       </c>
-      <c r="C27" s="8">
+      <c r="C27" s="2">
         <v>4.71</v>
       </c>
     </row>
@@ -1539,10 +1470,10 @@
       <c r="A28" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B28" s="8">
-        <v>0</v>
-      </c>
-      <c r="C28" s="8">
+      <c r="B28" s="2">
+        <v>0</v>
+      </c>
+      <c r="C28" s="2">
         <v>5.12</v>
       </c>
     </row>
@@ -1550,10 +1481,10 @@
       <c r="A29" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B29" s="8">
+      <c r="B29" s="2">
         <v>0.3</v>
       </c>
-      <c r="C29" s="8">
+      <c r="C29" s="2">
         <v>5.15</v>
       </c>
     </row>
@@ -1561,10 +1492,10 @@
       <c r="A30" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="8">
-        <v>0</v>
-      </c>
-      <c r="C30" s="8">
+      <c r="B30" s="2">
+        <v>0</v>
+      </c>
+      <c r="C30" s="2">
         <v>4.59</v>
       </c>
     </row>
@@ -1572,10 +1503,10 @@
       <c r="A31" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B31" s="8">
-        <v>0</v>
-      </c>
-      <c r="C31" s="8">
+      <c r="B31" s="2">
+        <v>0</v>
+      </c>
+      <c r="C31" s="2">
         <v>6.45</v>
       </c>
     </row>
@@ -1583,17 +1514,15 @@
       <c r="A32" s="3">
         <v>85558</v>
       </c>
-      <c r="B32" s="8"/>
-      <c r="C32" s="8"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B33" s="8">
-        <v>0</v>
-      </c>
-      <c r="C33" s="8">
+      <c r="B33" s="2">
+        <v>0</v>
+      </c>
+      <c r="C33" s="2">
         <v>5.94</v>
       </c>
     </row>
@@ -1601,10 +1530,10 @@
       <c r="A34" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B34" s="8">
+      <c r="B34" s="2">
         <v>0.1</v>
       </c>
-      <c r="C34" s="8">
+      <c r="C34" s="2">
         <v>5.57</v>
       </c>
     </row>
@@ -1612,10 +1541,10 @@
       <c r="A35" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="8">
-        <v>0</v>
-      </c>
-      <c r="C35" s="8">
+      <c r="B35" s="2">
+        <v>0</v>
+      </c>
+      <c r="C35" s="2">
         <v>5.85</v>
       </c>
     </row>
@@ -1623,10 +1552,10 @@
       <c r="A36" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B36" s="8">
+      <c r="B36" s="2">
         <v>0.5</v>
       </c>
-      <c r="C36" s="8">
+      <c r="C36" s="2">
         <v>5.69</v>
       </c>
     </row>
@@ -1634,10 +1563,10 @@
       <c r="A37" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B37" s="8">
-        <v>0</v>
-      </c>
-      <c r="C37" s="8">
+      <c r="B37" s="2">
+        <v>0</v>
+      </c>
+      <c r="C37" s="2">
         <v>6</v>
       </c>
     </row>
@@ -1645,10 +1574,10 @@
       <c r="A38" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B38" s="8">
-        <v>0</v>
-      </c>
-      <c r="C38" s="8">
+      <c r="B38" s="2">
+        <v>0</v>
+      </c>
+      <c r="C38" s="2">
         <v>6</v>
       </c>
     </row>
@@ -1656,17 +1585,15 @@
       <c r="A39" s="3">
         <v>49068</v>
       </c>
-      <c r="B39" s="8"/>
-      <c r="C39" s="8"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B40" s="8">
+      <c r="B40" s="2">
         <v>0.1</v>
       </c>
-      <c r="C40" s="8">
+      <c r="C40" s="2">
         <v>6</v>
       </c>
     </row>
@@ -1674,10 +1601,10 @@
       <c r="A41" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B41" s="8">
+      <c r="B41" s="2">
         <v>3</v>
       </c>
-      <c r="C41" s="8">
+      <c r="C41" s="2">
         <v>5.53</v>
       </c>
     </row>
@@ -1685,10 +1612,10 @@
       <c r="A42" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B42" s="8">
+      <c r="B42" s="2">
         <v>1</v>
       </c>
-      <c r="C42" s="8">
+      <c r="C42" s="2">
         <v>5.85</v>
       </c>
     </row>
@@ -1696,10 +1623,10 @@
       <c r="A43" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B43" s="8">
+      <c r="B43" s="2">
         <v>0.8</v>
       </c>
-      <c r="C43" s="8">
+      <c r="C43" s="2">
         <v>5.77</v>
       </c>
     </row>
@@ -1707,10 +1634,10 @@
       <c r="A44" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B44" s="8">
-        <v>0</v>
-      </c>
-      <c r="C44" s="8">
+      <c r="B44" s="2">
+        <v>0</v>
+      </c>
+      <c r="C44" s="2">
         <v>6</v>
       </c>
     </row>
@@ -1718,10 +1645,10 @@
       <c r="A45" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B45" s="8">
-        <v>0</v>
-      </c>
-      <c r="C45" s="8">
+      <c r="B45" s="2">
+        <v>0</v>
+      </c>
+      <c r="C45" s="2">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Finish instructions; Add image of results
</commit_message>
<xml_diff>
--- a/Post2026WebTool/DMDU-Performance.xlsx
+++ b/Post2026WebTool/DMDU-Performance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCollaborate\Post2026WebTool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74622766-8B5F-4CC0-A588-A1683F4088E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFC53CE0-3651-443B-B812-9D802567F6BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26370" yWindow="1155" windowWidth="21600" windowHeight="12525" activeTab="3" xr2:uid="{5F776126-F472-4954-8F54-2D1027C60DF9}"/>
+    <workbookView xWindow="-57720" yWindow="-1800" windowWidth="29040" windowHeight="17520" xr2:uid="{5F776126-F472-4954-8F54-2D1027C60DF9}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="25" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="58">
   <si>
     <t>Hydrology</t>
   </si>
@@ -210,6 +210,12 @@
   </si>
   <si>
     <t>CRB Post-2026 Tool</t>
+  </si>
+  <si>
+    <t>Strategies</t>
+  </si>
+  <si>
+    <t>Description of the 6 strategies included in the analysis.</t>
   </si>
 </sst>
 </file>
@@ -265,7 +271,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -298,21 +304,18 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{E7C15270-7CE4-4FD1-B902-B867009F5E38}"/>
   </cellStyles>
-  <dxfs count="68">
+  <dxfs count="4">
     <dxf>
       <alignment wrapText="1"/>
     </dxf>
@@ -324,198 +327,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -884,7 +695,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00E99385-38E0-4A97-8334-300435782A5C}" name="PivotTable1" cacheId="25" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00E99385-38E0-4A97-8334-300435782A5C}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C38" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
@@ -1054,10 +865,10 @@
     <dataField name="Sum of GCD Minimum Annual Release (maf)" fld="5" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="4">
-    <format dxfId="67">
+    <format dxfId="0">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0"/>
     </format>
-    <format dxfId="66">
+    <format dxfId="1">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="2">
@@ -1067,10 +878,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="65">
+    <format dxfId="2">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="64">
+    <format dxfId="3">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="2">
@@ -1410,10 +1221,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDE794B6-A7D0-4151-B3B3-0A01917D1254}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1461,6 +1272,14 @@
         <v>19</v>
       </c>
     </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1470,8 +1289,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADA64DF2-8BDA-4183-86B2-4FB89DC77176}">
   <dimension ref="A3:AG81"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView topLeftCell="A3" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1518,8 +1337,8 @@
       <c r="A4" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
       <c r="D4"/>
       <c r="E4"/>
       <c r="F4"/>
@@ -1555,10 +1374,10 @@
       <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="12">
-        <v>0</v>
-      </c>
-      <c r="C5" s="12">
+      <c r="B5" s="2">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2">
         <v>4.12</v>
       </c>
     </row>
@@ -1566,10 +1385,10 @@
       <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="12">
-        <v>0</v>
-      </c>
-      <c r="C6" s="12">
+      <c r="B6" s="2">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2">
         <v>3.97</v>
       </c>
     </row>
@@ -1577,10 +1396,10 @@
       <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="12">
-        <v>0</v>
-      </c>
-      <c r="C7" s="12">
+      <c r="B7" s="2">
+        <v>0</v>
+      </c>
+      <c r="C7" s="2">
         <v>4.1900000000000004</v>
       </c>
     </row>
@@ -1588,10 +1407,10 @@
       <c r="A8" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="12">
-        <v>0</v>
-      </c>
-      <c r="C8" s="12">
+      <c r="B8" s="2">
+        <v>0</v>
+      </c>
+      <c r="C8" s="2">
         <v>4.1100000000000003</v>
       </c>
     </row>
@@ -1599,10 +1418,10 @@
       <c r="A9" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="12">
-        <v>0</v>
-      </c>
-      <c r="C9" s="12">
+      <c r="B9" s="2">
+        <v>0</v>
+      </c>
+      <c r="C9" s="2">
         <v>3.96</v>
       </c>
     </row>
@@ -1610,10 +1429,10 @@
       <c r="A10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="12">
-        <v>0</v>
-      </c>
-      <c r="C10" s="12">
+      <c r="B10" s="2">
+        <v>0</v>
+      </c>
+      <c r="C10" s="2">
         <v>4.4800000000000004</v>
       </c>
     </row>
@@ -1621,17 +1440,15 @@
       <c r="A11" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="12">
-        <v>0</v>
-      </c>
-      <c r="C12" s="12">
+      <c r="B12" s="2">
+        <v>0</v>
+      </c>
+      <c r="C12" s="2">
         <v>4.74</v>
       </c>
     </row>
@@ -1639,10 +1456,10 @@
       <c r="A13" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="12">
-        <v>0</v>
-      </c>
-      <c r="C13" s="12">
+      <c r="B13" s="2">
+        <v>0</v>
+      </c>
+      <c r="C13" s="2">
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -1650,10 +1467,10 @@
       <c r="A14" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="12">
-        <v>0</v>
-      </c>
-      <c r="C14" s="12">
+      <c r="B14" s="2">
+        <v>0</v>
+      </c>
+      <c r="C14" s="2">
         <v>4.68</v>
       </c>
     </row>
@@ -1661,10 +1478,10 @@
       <c r="A15" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="12">
-        <v>0</v>
-      </c>
-      <c r="C15" s="12">
+      <c r="B15" s="2">
+        <v>0</v>
+      </c>
+      <c r="C15" s="2">
         <v>4.4400000000000004</v>
       </c>
     </row>
@@ -1672,10 +1489,10 @@
       <c r="A16" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="12">
-        <v>0</v>
-      </c>
-      <c r="C16" s="12">
+      <c r="B16" s="2">
+        <v>0</v>
+      </c>
+      <c r="C16" s="2">
         <v>4.2699999999999996</v>
       </c>
     </row>
@@ -1683,10 +1500,10 @@
       <c r="A17" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="12">
-        <v>0</v>
-      </c>
-      <c r="C17" s="12">
+      <c r="B17" s="2">
+        <v>0</v>
+      </c>
+      <c r="C17" s="2">
         <v>5.41</v>
       </c>
     </row>
@@ -1694,17 +1511,15 @@
       <c r="A18" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B19" s="12">
-        <v>0</v>
-      </c>
-      <c r="C19" s="12">
+      <c r="B19" s="2">
+        <v>0</v>
+      </c>
+      <c r="C19" s="2">
         <v>4.74</v>
       </c>
     </row>
@@ -1712,10 +1527,10 @@
       <c r="A20" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B20" s="12">
+      <c r="B20" s="2">
         <v>0.1</v>
       </c>
-      <c r="C20" s="12">
+      <c r="C20" s="2">
         <v>4.6100000000000003</v>
       </c>
     </row>
@@ -1723,10 +1538,10 @@
       <c r="A21" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="12">
-        <v>0</v>
-      </c>
-      <c r="C21" s="12">
+      <c r="B21" s="2">
+        <v>0</v>
+      </c>
+      <c r="C21" s="2">
         <v>4.6900000000000004</v>
       </c>
     </row>
@@ -1734,10 +1549,10 @@
       <c r="A22" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B22" s="12">
-        <v>0</v>
-      </c>
-      <c r="C22" s="12">
+      <c r="B22" s="2">
+        <v>0</v>
+      </c>
+      <c r="C22" s="2">
         <v>4.75</v>
       </c>
     </row>
@@ -1745,10 +1560,10 @@
       <c r="A23" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="12">
-        <v>0</v>
-      </c>
-      <c r="C23" s="12">
+      <c r="B23" s="2">
+        <v>0</v>
+      </c>
+      <c r="C23" s="2">
         <v>4.41</v>
       </c>
     </row>
@@ -1756,10 +1571,10 @@
       <c r="A24" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B24" s="12">
-        <v>0</v>
-      </c>
-      <c r="C24" s="12">
+      <c r="B24" s="2">
+        <v>0</v>
+      </c>
+      <c r="C24" s="2">
         <v>6.03</v>
       </c>
     </row>
@@ -1767,17 +1582,15 @@
       <c r="A25" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B25" s="12"/>
-      <c r="C25" s="12"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B26" s="12">
-        <v>0</v>
-      </c>
-      <c r="C26" s="12">
+      <c r="B26" s="2">
+        <v>0</v>
+      </c>
+      <c r="C26" s="2">
         <v>5.94</v>
       </c>
     </row>
@@ -1785,10 +1598,10 @@
       <c r="A27" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B27" s="12">
+      <c r="B27" s="2">
         <v>0.1</v>
       </c>
-      <c r="C27" s="12">
+      <c r="C27" s="2">
         <v>5.57</v>
       </c>
     </row>
@@ -1796,10 +1609,10 @@
       <c r="A28" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B28" s="12">
-        <v>0</v>
-      </c>
-      <c r="C28" s="12">
+      <c r="B28" s="2">
+        <v>0</v>
+      </c>
+      <c r="C28" s="2">
         <v>5.85</v>
       </c>
     </row>
@@ -1807,10 +1620,10 @@
       <c r="A29" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B29" s="12">
+      <c r="B29" s="2">
         <v>0.5</v>
       </c>
-      <c r="C29" s="12">
+      <c r="C29" s="2">
         <v>5.69</v>
       </c>
     </row>
@@ -1818,10 +1631,10 @@
       <c r="A30" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="12">
-        <v>0</v>
-      </c>
-      <c r="C30" s="12">
+      <c r="B30" s="2">
+        <v>0</v>
+      </c>
+      <c r="C30" s="2">
         <v>6</v>
       </c>
     </row>
@@ -1829,10 +1642,10 @@
       <c r="A31" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B31" s="12">
-        <v>0</v>
-      </c>
-      <c r="C31" s="12">
+      <c r="B31" s="2">
+        <v>0</v>
+      </c>
+      <c r="C31" s="2">
         <v>6</v>
       </c>
     </row>
@@ -1840,17 +1653,15 @@
       <c r="A32" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B32" s="12"/>
-      <c r="C32" s="12"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B33" s="12">
-        <v>0</v>
-      </c>
-      <c r="C33" s="12">
+      <c r="B33" s="2">
+        <v>0</v>
+      </c>
+      <c r="C33" s="2">
         <v>5.16</v>
       </c>
     </row>
@@ -1858,10 +1669,10 @@
       <c r="A34" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B34" s="12">
+      <c r="B34" s="2">
         <v>0.1</v>
       </c>
-      <c r="C34" s="12">
+      <c r="C34" s="2">
         <v>4.71</v>
       </c>
     </row>
@@ -1869,10 +1680,10 @@
       <c r="A35" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="12">
-        <v>0</v>
-      </c>
-      <c r="C35" s="12">
+      <c r="B35" s="2">
+        <v>0</v>
+      </c>
+      <c r="C35" s="2">
         <v>5.12</v>
       </c>
     </row>
@@ -1880,10 +1691,10 @@
       <c r="A36" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B36" s="12">
+      <c r="B36" s="2">
         <v>0.3</v>
       </c>
-      <c r="C36" s="12">
+      <c r="C36" s="2">
         <v>5.15</v>
       </c>
     </row>
@@ -1891,10 +1702,10 @@
       <c r="A37" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B37" s="12">
-        <v>0</v>
-      </c>
-      <c r="C37" s="12">
+      <c r="B37" s="2">
+        <v>0</v>
+      </c>
+      <c r="C37" s="2">
         <v>4.59</v>
       </c>
     </row>
@@ -1902,10 +1713,10 @@
       <c r="A38" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B38" s="12">
-        <v>0</v>
-      </c>
-      <c r="C38" s="12">
+      <c r="B38" s="2">
+        <v>0</v>
+      </c>
+      <c r="C38" s="2">
         <v>6.45</v>
       </c>
     </row>
@@ -2873,28 +2684,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6B9D69D-9A89-4A71-A09B-D666F7216ED8}">
   <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.81640625" style="13" customWidth="1"/>
-    <col min="2" max="2" width="6.7265625" style="13" customWidth="1"/>
-    <col min="3" max="3" width="21.6328125" style="13" customWidth="1"/>
-    <col min="4" max="4" width="36.453125" style="13" customWidth="1"/>
-    <col min="5" max="5" width="54" style="13" customWidth="1"/>
-    <col min="6" max="6" width="49.90625" style="13" customWidth="1"/>
-    <col min="7" max="9" width="47.26953125" style="13" customWidth="1"/>
-    <col min="10" max="10" width="45.90625" style="13" customWidth="1"/>
-    <col min="11" max="11" width="49.90625" style="13" customWidth="1"/>
-    <col min="12" max="12" width="44.54296875" style="13" customWidth="1"/>
-    <col min="13" max="13" width="39.1796875" style="13" customWidth="1"/>
-    <col min="14" max="16384" width="8.7265625" style="13"/>
+    <col min="1" max="1" width="14.81640625" style="12" customWidth="1"/>
+    <col min="2" max="2" width="6.7265625" style="12" customWidth="1"/>
+    <col min="3" max="3" width="21.6328125" style="12" customWidth="1"/>
+    <col min="4" max="4" width="36.453125" style="12" customWidth="1"/>
+    <col min="5" max="5" width="54" style="12" customWidth="1"/>
+    <col min="6" max="6" width="49.90625" style="12" customWidth="1"/>
+    <col min="7" max="9" width="47.26953125" style="12" customWidth="1"/>
+    <col min="10" max="10" width="45.90625" style="12" customWidth="1"/>
+    <col min="11" max="11" width="49.90625" style="12" customWidth="1"/>
+    <col min="12" max="12" width="44.54296875" style="12" customWidth="1"/>
+    <col min="13" max="13" width="39.1796875" style="12" customWidth="1"/>
+    <col min="14" max="16384" width="8.7265625" style="12"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="14" t="s">
         <v>55</v>
       </c>
       <c r="B1" s="15"/>
@@ -2911,176 +2722,176 @@
       <c r="M1" s="15"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="H2" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="I2" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="J2" s="14" t="s">
+      <c r="J2" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="K2" s="14" t="s">
+      <c r="K2" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="L2" s="14" t="s">
+      <c r="L2" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="M2" s="14" t="s">
+      <c r="M2" s="13" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="G3" s="13">
+      <c r="G3" s="12">
         <v>5.5</v>
       </c>
-      <c r="H3" s="13">
+      <c r="H3" s="12">
         <v>9.25</v>
       </c>
-      <c r="I3" s="13">
+      <c r="I3" s="12">
         <v>3700</v>
       </c>
-      <c r="K3" s="13">
+      <c r="K3" s="12">
         <v>80</v>
       </c>
-      <c r="M3" s="13">
+      <c r="M3" s="12">
         <v>3.4</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="G4" s="13">
+      <c r="G4" s="12">
         <v>6</v>
       </c>
-      <c r="H4" s="13">
+      <c r="H4" s="12">
         <v>10</v>
       </c>
-      <c r="I4" s="13">
+      <c r="I4" s="12">
         <v>3700</v>
       </c>
-      <c r="K4" s="13">
+      <c r="K4" s="12">
         <v>80</v>
       </c>
-      <c r="M4" s="13">
+      <c r="M4" s="12">
         <v>3.4</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="G5" s="13">
+      <c r="G5" s="12">
         <v>6</v>
       </c>
-      <c r="H5" s="13">
+      <c r="H5" s="12">
         <v>9</v>
       </c>
-      <c r="I5" s="13">
+      <c r="I5" s="12">
         <v>3670</v>
       </c>
-      <c r="K5" s="13">
+      <c r="K5" s="12">
         <v>70</v>
       </c>
-      <c r="M5" s="13">
+      <c r="M5" s="12">
         <v>3.9</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="13">
+      <c r="F6" s="12">
         <v>3</v>
       </c>
-      <c r="K6" s="13">
+      <c r="K6" s="12">
         <v>90</v>
       </c>
-      <c r="M6" s="13">
+      <c r="M6" s="12">
         <v>3.5</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="13">
+      <c r="F7" s="12">
         <v>1</v>
       </c>
-      <c r="K7" s="13">
+      <c r="K7" s="12">
         <v>90</v>
       </c>
-      <c r="M7" s="13">
+      <c r="M7" s="12">
         <v>3.5</v>
       </c>
     </row>

</xml_diff>